<commit_message>
Update conceptos de data género.xlsx
</commit_message>
<xml_diff>
--- a/conceptos de data género.xlsx
+++ b/conceptos de data género.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvcma\Dropbox\Diseño DATA's\DATA-GENERO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA INTELLIGENCE Dropbox\Diseño DATA's\DATA-GENERO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D62C20B-D39F-46E6-ADD5-9EF4A2604925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23ED8D8D-E199-4981-8E21-10158EDAF634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{67760E13-AA5E-456D-9C09-F0A843BE1AB5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{67760E13-AA5E-456D-9C09-F0A843BE1AB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -432,11 +432,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -755,23 +755,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B84E7B5-9EC9-42DA-B4D4-C16593594ACF}">
   <dimension ref="B3:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="99.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="99.109375" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -779,7 +779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
@@ -790,7 +790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -801,7 +801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="140.4" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
@@ -812,7 +812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="218.4" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
@@ -823,7 +823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="189" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="C10" s="8" t="s">
         <v>12</v>
       </c>
@@ -834,7 +834,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="C11" s="10" t="s">
         <v>15</v>
       </c>
@@ -845,7 +845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
@@ -856,7 +856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="78" x14ac:dyDescent="0.3">
       <c r="C13" s="10" t="s">
         <v>20</v>
       </c>
@@ -867,7 +867,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="267.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="234" x14ac:dyDescent="0.3">
       <c r="C14" s="10" t="s">
         <v>22</v>
       </c>
@@ -878,15 +878,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="2"/>

</xml_diff>